<commit_message>
Initial commit for car + highway.json
</commit_message>
<xml_diff>
--- a/FinalProject/layout_note.xlsx
+++ b/FinalProject/layout_note.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="491" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="223" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="small" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="lombard" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="highway" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="79">
   <si>
     <t>col</t>
   </si>
@@ -241,6 +242,18 @@
   </si>
   <si>
     <t>29E</t>
+  </si>
+  <si>
+    <t>2S</t>
+  </si>
+  <si>
+    <t>3S</t>
+  </si>
+  <si>
+    <t>0N</t>
+  </si>
+  <si>
+    <t>4N</t>
   </si>
 </sst>
 </file>
@@ -334,7 +347,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -357,6 +370,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1503,8 +1520,8 @@
   </sheetPr>
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1521,6 +1538,17 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -1530,6 +1558,32 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
@@ -2491,16 +2545,52 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
+      <c r="B30" s="0"/>
+      <c r="C30" s="0"/>
+      <c r="D30" s="0"/>
+      <c r="E30" s="0"/>
+      <c r="F30" s="0"/>
+      <c r="G30" s="0"/>
+      <c r="H30" s="0"/>
+      <c r="I30" s="0"/>
+      <c r="J30" s="0"/>
+      <c r="K30" s="0"/>
+      <c r="L30" s="0"/>
+      <c r="M30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B31" s="0"/>
+      <c r="C31" s="0"/>
+      <c r="D31" s="0"/>
+      <c r="E31" s="0"/>
+      <c r="F31" s="0"/>
+      <c r="G31" s="0"/>
+      <c r="H31" s="0"/>
+      <c r="I31" s="0"/>
+      <c r="J31" s="0"/>
+      <c r="K31" s="0"/>
+      <c r="L31" s="0"/>
+      <c r="M31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B32" s="0"/>
+      <c r="C32" s="0"/>
+      <c r="D32" s="0"/>
+      <c r="E32" s="0"/>
+      <c r="F32" s="0"/>
+      <c r="G32" s="0"/>
+      <c r="H32" s="0"/>
+      <c r="I32" s="0"/>
+      <c r="J32" s="0"/>
+      <c r="K32" s="0"/>
+      <c r="L32" s="0"/>
+      <c r="M32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3"/>
@@ -3068,4 +3158,703 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G57"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="11" min="1" style="2" width="3.88775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="2" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="n">
+        <f aca="false">120/30</f>
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <f aca="false">720/30</f>
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <f aca="false">B5+1</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <f aca="false">C5+1</f>
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <f aca="false">D5+1</f>
+        <v>4</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
+        <f aca="false">A6+1</f>
+        <v>2</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="n">
+        <f aca="false">A7+1</f>
+        <v>3</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="n">
+        <f aca="false">A8+1</f>
+        <v>4</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="n">
+        <f aca="false">A9+1</f>
+        <v>5</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="n">
+        <f aca="false">A10+1</f>
+        <v>6</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="n">
+        <f aca="false">A11+1</f>
+        <v>7</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="n">
+        <f aca="false">A12+1</f>
+        <v>8</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="n">
+        <f aca="false">A13+1</f>
+        <v>9</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="n">
+        <f aca="false">A14+1</f>
+        <v>10</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="n">
+        <f aca="false">A15+1</f>
+        <v>11</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="n">
+        <f aca="false">A16+1</f>
+        <v>12</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="n">
+        <f aca="false">A17+1</f>
+        <v>13</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="n">
+        <f aca="false">A18+1</f>
+        <v>14</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="n">
+        <f aca="false">A19+1</f>
+        <v>15</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="n">
+        <f aca="false">A20+1</f>
+        <v>16</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="n">
+        <f aca="false">A21+1</f>
+        <v>17</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="n">
+        <f aca="false">A22+1</f>
+        <v>18</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="n">
+        <f aca="false">A23+1</f>
+        <v>19</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="n">
+        <f aca="false">A24+1</f>
+        <v>20</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="n">
+        <f aca="false">A25+1</f>
+        <v>21</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="n">
+        <f aca="false">A26+1</f>
+        <v>22</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="n">
+        <f aca="false">A27+1</f>
+        <v>23</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="n">
+        <f aca="false">A28+1</f>
+        <v>24</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3" t="n">
+        <f aca="false">B33+1</f>
+        <v>2</v>
+      </c>
+      <c r="D33" s="3" t="n">
+        <f aca="false">C33+1</f>
+        <v>3</v>
+      </c>
+      <c r="E33" s="3" t="n">
+        <f aca="false">D33+1</f>
+        <v>4</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="n">
+        <f aca="false">A34+1</f>
+        <v>2</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="n">
+        <f aca="false">A35+1</f>
+        <v>3</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="n">
+        <f aca="false">A36+1</f>
+        <v>4</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="n">
+        <f aca="false">A37+1</f>
+        <v>5</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="0"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="n">
+        <f aca="false">A38+1</f>
+        <v>6</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="n">
+        <f aca="false">A39+1</f>
+        <v>7</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="n">
+        <f aca="false">A40+1</f>
+        <v>8</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="n">
+        <f aca="false">A41+1</f>
+        <v>9</v>
+      </c>
+      <c r="B42" s="4"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="n">
+        <f aca="false">A42+1</f>
+        <v>10</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3" t="n">
+        <f aca="false">A43+1</f>
+        <v>11</v>
+      </c>
+      <c r="B44" s="4"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="3" t="n">
+        <f aca="false">A44+1</f>
+        <v>12</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="3" t="n">
+        <f aca="false">A45+1</f>
+        <v>13</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="3" t="n">
+        <f aca="false">A46+1</f>
+        <v>14</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="3" t="n">
+        <f aca="false">A47+1</f>
+        <v>15</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="3" t="n">
+        <f aca="false">A48+1</f>
+        <v>16</v>
+      </c>
+      <c r="B49" s="4"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="3" t="n">
+        <f aca="false">A49+1</f>
+        <v>17</v>
+      </c>
+      <c r="B50" s="4"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="3" t="n">
+        <f aca="false">A50+1</f>
+        <v>18</v>
+      </c>
+      <c r="B51" s="4"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3" t="n">
+        <f aca="false">A51+1</f>
+        <v>19</v>
+      </c>
+      <c r="B52" s="4"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="3" t="n">
+        <f aca="false">A52+1</f>
+        <v>20</v>
+      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="3" t="n">
+        <f aca="false">A53+1</f>
+        <v>21</v>
+      </c>
+      <c r="B54" s="4"/>
+      <c r="C54" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E54" s="4"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="n">
+        <f aca="false">A54+1</f>
+        <v>22</v>
+      </c>
+      <c r="B55" s="4"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="3" t="n">
+        <f aca="false">A55+1</f>
+        <v>23</v>
+      </c>
+      <c r="B56" s="4"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E56" s="4"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="3" t="n">
+        <f aca="false">A56+1</f>
+        <v>24</v>
+      </c>
+      <c r="B57" s="4"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>